<commit_message>
server: db class 함수 수정
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Mode_Ver3.xlsx
+++ b/Server/Server/GameData/Mode_Ver3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\porject\기획서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0753B07C-4FA4-4765-88E2-ADF01BFBD2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D730145-55D7-43AE-8610-4044A557A548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="490" activeTab="2" xr2:uid="{00881117-46AD-47BC-AC4E-DE2587EC70E9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="490" activeTab="2" xr2:uid="{00881117-46AD-47BC-AC4E-DE2587EC70E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Matching" sheetId="10" r:id="rId1"/>
@@ -1905,7 +1905,8 @@
   <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2097,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="U2">
         <v>2002</v>
@@ -2106,31 +2107,31 @@
         <v>1</v>
       </c>
       <c r="W2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="X2">
         <v>3001</v>
       </c>
       <c r="Y2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Z2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AA2">
         <v>3002</v>
       </c>
       <c r="AB2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AC2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>11102</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="U3">
         <v>2002</v>
@@ -2198,31 +2199,31 @@
         <v>1</v>
       </c>
       <c r="W3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="X3">
         <v>3001</v>
       </c>
       <c r="Y3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Z3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AA3">
         <v>3002</v>
       </c>
       <c r="AB3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AC3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>11103</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="T4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="U4">
         <v>2002</v>
@@ -2290,31 +2291,31 @@
         <v>1</v>
       </c>
       <c r="W4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="X4">
         <v>3001</v>
       </c>
       <c r="Y4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Z4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AA4">
         <v>3002</v>
       </c>
       <c r="AB4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AC4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>11201</v>
       </c>
@@ -2382,13 +2383,13 @@
         <v>1</v>
       </c>
       <c r="W5">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X5">
         <v>3001</v>
       </c>
       <c r="Y5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Z5">
         <v>10</v>
@@ -2397,16 +2398,16 @@
         <v>3002</v>
       </c>
       <c r="AB5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AC5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>12101</v>
       </c>
@@ -2480,7 +2481,7 @@
         <v>3001</v>
       </c>
       <c r="Y6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Z6">
         <v>10</v>
@@ -2489,16 +2490,16 @@
         <v>3002</v>
       </c>
       <c r="AB6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>12102</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>3001</v>
       </c>
       <c r="Y7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Z7">
         <v>10</v>
@@ -2581,16 +2582,16 @@
         <v>3002</v>
       </c>
       <c r="AB7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>12201</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>3001</v>
       </c>
       <c r="Y8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Z8">
         <v>10</v>
@@ -2673,16 +2674,16 @@
         <v>3002</v>
       </c>
       <c r="AB8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>12202</v>
       </c>
@@ -2756,7 +2757,7 @@
         <v>3001</v>
       </c>
       <c r="Y9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Z9">
         <v>10</v>
@@ -2765,19 +2766,16 @@
         <v>3002</v>
       </c>
       <c r="AB9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD9">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="I15" t="s">
         <v>46</v>
       </c>

</xml_diff>